<commit_message>
Updates example inputs and merging
</commit_message>
<xml_diff>
--- a/inputs/CA Intertidal Barcode Data Received Updated 08062025.xlsx
+++ b/inputs/CA Intertidal Barcode Data Received Updated 08062025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcallister/software/scripts/github/OMISSION/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA9902F-A318-E341-8712-2829B36E5EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD75C02A-1F9A-A142-B60D-A234DC2F29B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12300" yWindow="-19580" windowWidth="40040" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7760" yWindow="-24900" windowWidth="40040" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recevied from Form" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -420,6 +420,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,7 +644,7 @@
   <dimension ref="A1:AG925"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -744,7 +747,7 @@
       <c r="H2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="J2" s="6" t="s">

</xml_diff>